<commit_message>
Add build-cfg.js - generate agentless.cfg and app_dev_id.cfg
</commit_message>
<xml_diff>
--- a/15C-Red-BOM-2015-08-07.xlsx
+++ b/15C-Red-BOM-2015-08-07.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26408"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbothwell/Documents/Git/jar-verify/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="320" windowWidth="24100" windowHeight="16520"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="24100" windowHeight="16520"/>
   </bookViews>
   <sheets>
     <sheet name="UX Package Info" sheetId="5" r:id="rId1"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="401">
   <si>
     <t>Operating Systems</t>
   </si>
@@ -1448,14 +1453,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Vendor ID: 10DF
-Device ID: E200</t>
-  </si>
-  <si>
-    <t>Vendor ID: 10DF
-Device ID: 0720</t>
   </si>
 </sst>
 </file>
@@ -1705,9 +1702,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="144">
+  <cellStyleXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2142,6 +2141,46 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2154,12 +2193,6 @@
     <xf numFmtId="16" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2181,51 +2214,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="144">
+  <cellStyles count="146">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2297,6 +2296,7 @@
     <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2368,6 +2368,7 @@
     <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -2670,11 +2671,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="2"/>
     <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
@@ -2704,53 +2705,53 @@
     <col min="26" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18">
-      <c r="A1" s="134" t="s">
+    <row r="1" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="110" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="134"/>
-    </row>
-    <row r="2" spans="1:27" ht="18">
-      <c r="A2" s="134" t="s">
+      <c r="B1" s="110"/>
+    </row>
+    <row r="2" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="110" t="s">
         <v>397</v>
       </c>
-      <c r="B2" s="134"/>
-    </row>
-    <row r="4" spans="1:27" ht="15">
+      <c r="B2" s="110"/>
+    </row>
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="132" t="s">
+      <c r="D4" s="120" t="s">
         <v>398</v>
       </c>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="129" t="s">
+      <c r="H4" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="130"/>
-      <c r="J4" s="130"/>
-      <c r="K4" s="130"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="135"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
       <c r="N4" s="14"/>
-      <c r="O4" s="129" t="s">
+      <c r="O4" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="130"/>
-      <c r="Q4" s="130"/>
-      <c r="R4" s="130"/>
-      <c r="S4" s="130"/>
-      <c r="T4" s="130"/>
-      <c r="U4" s="130"/>
-      <c r="V4" s="130"/>
-      <c r="W4" s="130"/>
-      <c r="X4" s="130"/>
-      <c r="Y4" s="131"/>
-    </row>
-    <row r="5" spans="1:27">
+      <c r="P4" s="118"/>
+      <c r="Q4" s="118"/>
+      <c r="R4" s="118"/>
+      <c r="S4" s="118"/>
+      <c r="T4" s="118"/>
+      <c r="U4" s="118"/>
+      <c r="V4" s="118"/>
+      <c r="W4" s="118"/>
+      <c r="X4" s="118"/>
+      <c r="Y4" s="119"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B5" s="88" t="s">
         <v>48</v>
       </c>
@@ -2765,22 +2766,22 @@
         <v>6</v>
       </c>
       <c r="G5" s="19"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="136" t="s">
         <v>177</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="136" t="s">
         <v>399</v>
       </c>
       <c r="N5" s="20"/>
@@ -2818,24 +2819,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B6" s="89" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="123" t="s">
+      <c r="D6" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="124"/>
-      <c r="F6" s="125"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="116"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="123" t="s">
+      <c r="H6" s="137" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="125"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="137"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="137"/>
       <c r="M6" s="137"/>
       <c r="N6" s="24"/>
       <c r="O6" s="97" t="s">
@@ -2874,7 +2875,7 @@
       <c r="Z6" s="76"/>
       <c r="AA6" s="25"/>
     </row>
-    <row r="7" spans="1:27" ht="28">
+    <row r="7" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B7" s="90" t="s">
         <v>378</v>
       </c>
@@ -2944,7 +2945,7 @@
       <c r="Z7" s="76"/>
       <c r="AA7" s="32"/>
     </row>
-    <row r="8" spans="1:27" ht="28">
+    <row r="8" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B8" s="90" t="s">
         <v>379</v>
       </c>
@@ -3011,7 +3012,7 @@
       <c r="Z8" s="76"/>
       <c r="AA8" s="32"/>
     </row>
-    <row r="9" spans="1:27" ht="28">
+    <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B9" s="92" t="s">
         <v>380</v>
       </c>
@@ -3078,7 +3079,7 @@
       <c r="Z9" s="76"/>
       <c r="AA9" s="32"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B10" s="90" t="s">
         <v>381</v>
       </c>
@@ -3125,7 +3126,7 @@
       <c r="Z10" s="76"/>
       <c r="AA10" s="32"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B11" s="92" t="s">
         <v>382</v>
       </c>
@@ -3140,14 +3141,14 @@
         <v>5</v>
       </c>
       <c r="G11" s="39"/>
-      <c r="H11" s="123" t="s">
+      <c r="H11" s="137" t="s">
         <v>206</v>
       </c>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="125"/>
-      <c r="M11" s="136"/>
+      <c r="I11" s="137"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="137"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="137"/>
       <c r="O11" s="64" t="s">
         <v>276</v>
       </c>
@@ -3180,7 +3181,7 @@
       <c r="Z11" s="76"/>
       <c r="AA11" s="32"/>
     </row>
-    <row r="12" spans="1:27" ht="28">
+    <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B12" s="90" t="s">
         <v>383</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="114" t="s">
+      <c r="H12" s="121" t="s">
         <v>320</v>
       </c>
       <c r="I12" s="95" t="s">
@@ -3210,8 +3211,8 @@
       <c r="L12" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="M12" s="95" t="s">
-        <v>401</v>
+      <c r="M12" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O12" s="41" t="s">
         <v>286</v>
@@ -3242,7 +3243,7 @@
       <c r="Z12" s="76"/>
       <c r="AA12" s="32"/>
     </row>
-    <row r="13" spans="1:27" ht="28">
+    <row r="13" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B13" s="90" t="s">
         <v>384</v>
       </c>
@@ -3257,7 +3258,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="30"/>
-      <c r="H13" s="133"/>
+      <c r="H13" s="122"/>
       <c r="I13" s="95" t="s">
         <v>182</v>
       </c>
@@ -3270,8 +3271,8 @@
       <c r="L13" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="M13" s="95" t="s">
-        <v>401</v>
+      <c r="M13" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O13" s="41" t="s">
         <v>287</v>
@@ -3302,12 +3303,12 @@
       <c r="Z13" s="76"/>
       <c r="AA13" s="32"/>
     </row>
-    <row r="14" spans="1:27" ht="28">
+    <row r="14" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B14" s="90" t="s">
         <v>385</v>
       </c>
       <c r="C14" s="43"/>
-      <c r="H14" s="133"/>
+      <c r="H14" s="122"/>
       <c r="I14" s="105" t="s">
         <v>186</v>
       </c>
@@ -3320,8 +3321,8 @@
       <c r="L14" s="105" t="s">
         <v>181</v>
       </c>
-      <c r="M14" s="95" t="s">
-        <v>401</v>
+      <c r="M14" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O14" s="41" t="s">
         <v>288</v>
@@ -3353,17 +3354,17 @@
       <c r="Z14" s="76"/>
       <c r="AA14" s="32"/>
     </row>
-    <row r="15" spans="1:27" ht="28">
+    <row r="15" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="92" t="s">
         <v>386</v>
       </c>
       <c r="C15" s="43"/>
-      <c r="D15" s="126" t="s">
+      <c r="D15" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="E15" s="127"/>
-      <c r="F15" s="128"/>
-      <c r="H15" s="115"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="113"/>
+      <c r="H15" s="123"/>
       <c r="I15" s="95" t="s">
         <v>188</v>
       </c>
@@ -3376,8 +3377,8 @@
       <c r="L15" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="M15" s="95" t="s">
-        <v>401</v>
+      <c r="M15" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O15" s="97" t="s">
         <v>68</v>
@@ -3406,7 +3407,7 @@
       <c r="Z15" s="76"/>
       <c r="AA15" s="32"/>
     </row>
-    <row r="16" spans="1:27" ht="28">
+    <row r="16" spans="1:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B16" s="92" t="s">
         <v>387</v>
       </c>
@@ -3420,7 +3421,7 @@
       <c r="F16" s="45">
         <v>8</v>
       </c>
-      <c r="H16" s="114" t="s">
+      <c r="H16" s="121" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="40" t="s">
@@ -3435,8 +3436,8 @@
       <c r="L16" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="M16" s="95" t="s">
-        <v>401</v>
+      <c r="M16" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O16" s="97" t="s">
         <v>69</v>
@@ -3464,7 +3465,7 @@
       <c r="Z16" s="76"/>
       <c r="AA16" s="32"/>
     </row>
-    <row r="17" spans="2:27" ht="28">
+    <row r="17" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B17" s="91" t="s">
         <v>388</v>
       </c>
@@ -3479,7 +3480,7 @@
         <v>9</v>
       </c>
       <c r="G17" s="76"/>
-      <c r="H17" s="115"/>
+      <c r="H17" s="123"/>
       <c r="I17" s="40" t="s">
         <v>259</v>
       </c>
@@ -3492,8 +3493,8 @@
       <c r="L17" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="M17" s="95" t="s">
-        <v>401</v>
+      <c r="M17" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O17" s="97" t="s">
         <v>70</v>
@@ -3521,7 +3522,7 @@
       <c r="Z17" s="76"/>
       <c r="AA17" s="32"/>
     </row>
-    <row r="18" spans="2:27" ht="28">
+    <row r="18" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B18" s="90" t="s">
         <v>389</v>
       </c>
@@ -3536,7 +3537,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="76"/>
-      <c r="H18" s="116" t="s">
+      <c r="H18" s="128" t="s">
         <v>318</v>
       </c>
       <c r="I18" s="40" t="s">
@@ -3551,8 +3552,8 @@
       <c r="L18" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="M18" s="95" t="s">
-        <v>401</v>
+      <c r="M18" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O18" s="97" t="s">
         <v>370</v>
@@ -3581,7 +3582,7 @@
       <c r="Z18" s="76"/>
       <c r="AA18" s="32"/>
     </row>
-    <row r="19" spans="2:27" ht="28">
+    <row r="19" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B19" s="91" t="s">
         <v>390</v>
       </c>
@@ -3596,7 +3597,7 @@
         <v>11</v>
       </c>
       <c r="G19" s="76"/>
-      <c r="H19" s="117"/>
+      <c r="H19" s="129"/>
       <c r="I19" s="40" t="s">
         <v>261</v>
       </c>
@@ -3609,8 +3610,8 @@
       <c r="L19" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="M19" s="95" t="s">
-        <v>401</v>
+      <c r="M19" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O19" s="97" t="s">
         <v>371</v>
@@ -3638,7 +3639,7 @@
       </c>
       <c r="Z19" s="76"/>
     </row>
-    <row r="20" spans="2:27">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B20" s="90" t="s">
         <v>391</v>
       </c>
@@ -3673,21 +3674,21 @@
       </c>
       <c r="Z20" s="76"/>
     </row>
-    <row r="21" spans="2:27">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B21" s="92" t="s">
         <v>392</v>
       </c>
       <c r="C21" s="8"/>
       <c r="E21" s="7"/>
       <c r="F21" s="48"/>
-      <c r="H21" s="123" t="s">
+      <c r="H21" s="137" t="s">
         <v>207</v>
       </c>
-      <c r="I21" s="124"/>
-      <c r="J21" s="124"/>
-      <c r="K21" s="124"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="136"/>
+      <c r="I21" s="137"/>
+      <c r="J21" s="137"/>
+      <c r="K21" s="137"/>
+      <c r="L21" s="137"/>
+      <c r="M21" s="137"/>
       <c r="O21" s="97" t="s">
         <v>74</v>
       </c>
@@ -3707,14 +3708,14 @@
       </c>
       <c r="Z21" s="76"/>
     </row>
-    <row r="22" spans="2:27" ht="42">
+    <row r="22" spans="2:27" ht="45" x14ac:dyDescent="0.2">
       <c r="B22" s="92" t="s">
         <v>393</v>
       </c>
       <c r="C22" s="8"/>
       <c r="E22" s="7"/>
       <c r="F22" s="48"/>
-      <c r="H22" s="118" t="s">
+      <c r="H22" s="130" t="s">
         <v>320</v>
       </c>
       <c r="I22" s="95" t="s">
@@ -3752,14 +3753,14 @@
       </c>
       <c r="Z22" s="76"/>
     </row>
-    <row r="23" spans="2:27" ht="42">
+    <row r="23" spans="2:27" ht="45" x14ac:dyDescent="0.2">
       <c r="B23" s="90" t="s">
         <v>394</v>
       </c>
       <c r="C23" s="8"/>
       <c r="E23" s="7"/>
       <c r="F23" s="48"/>
-      <c r="H23" s="119"/>
+      <c r="H23" s="131"/>
       <c r="I23" s="95" t="s">
         <v>193</v>
       </c>
@@ -3795,7 +3796,7 @@
       </c>
       <c r="Z23" s="76"/>
     </row>
-    <row r="24" spans="2:27" ht="42">
+    <row r="24" spans="2:27" ht="45" x14ac:dyDescent="0.2">
       <c r="B24" s="92" t="s">
         <v>395</v>
       </c>
@@ -3841,7 +3842,7 @@
       </c>
       <c r="Z24" s="76"/>
     </row>
-    <row r="25" spans="2:27" ht="28">
+    <row r="25" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B25" s="90" t="s">
         <v>233</v>
       </c>
@@ -3868,21 +3869,21 @@
       </c>
       <c r="Z25" s="76"/>
     </row>
-    <row r="26" spans="2:27" ht="28">
+    <row r="26" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B26" s="50" t="s">
         <v>348</v>
       </c>
       <c r="D26" s="46"/>
       <c r="E26" s="7"/>
       <c r="F26" s="48"/>
-      <c r="H26" s="123" t="s">
+      <c r="H26" s="137" t="s">
         <v>208</v>
       </c>
-      <c r="I26" s="124"/>
-      <c r="J26" s="124"/>
-      <c r="K26" s="124"/>
-      <c r="L26" s="125"/>
-      <c r="M26" s="136"/>
+      <c r="I26" s="137"/>
+      <c r="J26" s="137"/>
+      <c r="K26" s="137"/>
+      <c r="L26" s="137"/>
+      <c r="M26" s="137"/>
       <c r="O26" s="97" t="s">
         <v>375</v>
       </c>
@@ -3904,13 +3905,13 @@
       </c>
       <c r="Z26" s="76"/>
     </row>
-    <row r="27" spans="2:27" ht="28">
+    <row r="27" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="B27" s="92" t="s">
         <v>357</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="48"/>
-      <c r="H27" s="120" t="s">
+      <c r="H27" s="132" t="s">
         <v>320</v>
       </c>
       <c r="I27" s="95" t="s">
@@ -3946,11 +3947,11 @@
       </c>
       <c r="Z27" s="76"/>
     </row>
-    <row r="28" spans="2:27" ht="28">
+    <row r="28" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="D28" s="71"/>
       <c r="E28" s="67"/>
       <c r="F28" s="72"/>
-      <c r="H28" s="121"/>
+      <c r="H28" s="133"/>
       <c r="I28" s="96" t="s">
         <v>334</v>
       </c>
@@ -3984,11 +3985,11 @@
       </c>
       <c r="Z28" s="76"/>
     </row>
-    <row r="29" spans="2:27" ht="28">
+    <row r="29" spans="2:27" ht="30" x14ac:dyDescent="0.2">
       <c r="D29" s="71"/>
       <c r="E29" s="67"/>
       <c r="F29" s="72"/>
-      <c r="H29" s="121"/>
+      <c r="H29" s="133"/>
       <c r="I29" s="95" t="s">
         <v>204</v>
       </c>
@@ -4021,12 +4022,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="30" spans="2:27" s="66" customFormat="1" ht="28">
+    <row r="30" spans="2:27" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="D30" s="46"/>
       <c r="E30" s="7"/>
       <c r="F30" s="48"/>
-      <c r="H30" s="121"/>
+      <c r="H30" s="133"/>
       <c r="I30" s="96" t="s">
         <v>343</v>
       </c>
@@ -4039,8 +4040,8 @@
       <c r="L30" s="95" t="s">
         <v>332</v>
       </c>
-      <c r="M30" s="95" t="s">
-        <v>402</v>
+      <c r="M30" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O30" s="97" t="s">
         <v>83</v>
@@ -4059,12 +4060,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="31" spans="2:27" s="66" customFormat="1" ht="28">
+    <row r="31" spans="2:27" s="66" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="D31" s="46"/>
       <c r="E31" s="7"/>
       <c r="F31" s="48"/>
-      <c r="H31" s="122"/>
+      <c r="H31" s="134"/>
       <c r="I31" s="96" t="s">
         <v>61</v>
       </c>
@@ -4077,8 +4078,8 @@
       <c r="L31" s="95" t="s">
         <v>346</v>
       </c>
-      <c r="M31" s="95" t="s">
-        <v>402</v>
+      <c r="M31" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O31" s="97" t="s">
         <v>84</v>
@@ -4097,11 +4098,11 @@
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="2:27" ht="56">
+    <row r="32" spans="2:27" ht="60" x14ac:dyDescent="0.2">
       <c r="D32" s="46"/>
       <c r="E32" s="7"/>
       <c r="F32" s="48"/>
-      <c r="H32" s="110" t="s">
+      <c r="H32" s="124" t="s">
         <v>356</v>
       </c>
       <c r="I32" s="96" t="s">
@@ -4135,11 +4136,11 @@
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="4:25" ht="28">
+    <row r="33" spans="4:25" ht="30" x14ac:dyDescent="0.2">
       <c r="D33" s="46"/>
       <c r="E33" s="7"/>
       <c r="F33" s="48"/>
-      <c r="H33" s="111"/>
+      <c r="H33" s="125"/>
       <c r="I33" s="96" t="s">
         <v>328</v>
       </c>
@@ -4152,8 +4153,8 @@
       <c r="L33" s="95" t="s">
         <v>344</v>
       </c>
-      <c r="M33" s="95" t="s">
-        <v>402</v>
+      <c r="M33" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="N33" s="25"/>
       <c r="O33" s="97" t="s">
@@ -4170,7 +4171,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="34" spans="4:25" ht="28">
+    <row r="34" spans="4:25" ht="30" x14ac:dyDescent="0.2">
       <c r="D34" s="46"/>
       <c r="E34" s="7"/>
       <c r="F34" s="48"/>
@@ -4208,11 +4209,11 @@
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="4:25" ht="28">
+    <row r="35" spans="4:25" ht="30" x14ac:dyDescent="0.2">
       <c r="D35" s="46"/>
       <c r="E35" s="7"/>
       <c r="F35" s="48"/>
-      <c r="H35" s="112" t="s">
+      <c r="H35" s="126" t="s">
         <v>347</v>
       </c>
       <c r="I35" s="96" t="s">
@@ -4227,8 +4228,8 @@
       <c r="L35" s="99" t="s">
         <v>301</v>
       </c>
-      <c r="M35" s="95" t="s">
-        <v>402</v>
+      <c r="M35" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O35" s="97" t="s">
         <v>353</v>
@@ -4246,11 +4247,11 @@
         <v>316</v>
       </c>
     </row>
-    <row r="36" spans="4:25" ht="30" customHeight="1">
+    <row r="36" spans="4:25" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="51"/>
       <c r="E36" s="6"/>
       <c r="F36" s="52"/>
-      <c r="H36" s="113"/>
+      <c r="H36" s="127"/>
       <c r="I36" s="96" t="s">
         <v>296</v>
       </c>
@@ -4263,8 +4264,8 @@
       <c r="L36" s="99" t="s">
         <v>302</v>
       </c>
-      <c r="M36" s="95" t="s">
-        <v>402</v>
+      <c r="M36" s="80" t="s">
+        <v>400</v>
       </c>
       <c r="O36" s="64" t="s">
         <v>277</v>
@@ -4282,7 +4283,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="4:25" ht="28">
+    <row r="37" spans="4:25" ht="30" x14ac:dyDescent="0.2">
       <c r="D37" s="51"/>
       <c r="E37" s="7"/>
       <c r="F37" s="52"/>
@@ -4319,7 +4320,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="38" spans="4:25" ht="28">
+    <row r="38" spans="4:25" ht="30" x14ac:dyDescent="0.2">
       <c r="H38" s="82">
         <v>11</v>
       </c>
@@ -4354,7 +4355,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="39" spans="4:25">
+    <row r="39" spans="4:25" x14ac:dyDescent="0.2">
       <c r="O39" s="97" t="s">
         <v>311</v>
       </c>
@@ -4371,7 +4372,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="40" spans="4:25">
+    <row r="40" spans="4:25" x14ac:dyDescent="0.2">
       <c r="O40" s="97" t="s">
         <v>312</v>
       </c>
@@ -4388,7 +4389,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="41" spans="4:25">
+    <row r="41" spans="4:25" x14ac:dyDescent="0.2">
       <c r="O41" s="97" t="s">
         <v>313</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="4:25">
+    <row r="42" spans="4:25" x14ac:dyDescent="0.2">
       <c r="H42" s="70"/>
       <c r="I42" s="66"/>
       <c r="J42" s="66"/>
@@ -4426,7 +4427,7 @@
       <c r="X42" s="42"/>
       <c r="Y42" s="25"/>
     </row>
-    <row r="43" spans="4:25">
+    <row r="43" spans="4:25" x14ac:dyDescent="0.2">
       <c r="O43" s="97" t="s">
         <v>315</v>
       </c>
@@ -4443,7 +4444,7 @@
       <c r="X43" s="42"/>
       <c r="Y43" s="25"/>
     </row>
-    <row r="44" spans="4:25">
+    <row r="44" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D44" s="54"/>
       <c r="E44" s="54"/>
       <c r="F44" s="54"/>
@@ -4467,7 +4468,7 @@
       <c r="X44" s="42"/>
       <c r="Y44" s="25"/>
     </row>
-    <row r="45" spans="4:25">
+    <row r="45" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D45" s="55"/>
       <c r="E45" s="56"/>
       <c r="F45" s="57"/>
@@ -4487,7 +4488,7 @@
       <c r="X45" s="42"/>
       <c r="Y45" s="25"/>
     </row>
-    <row r="46" spans="4:25">
+    <row r="46" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D46" s="55"/>
       <c r="E46" s="56"/>
       <c r="F46" s="57"/>
@@ -4507,7 +4508,7 @@
       <c r="X46" s="42"/>
       <c r="Y46" s="25"/>
     </row>
-    <row r="47" spans="4:25" ht="32.25" customHeight="1">
+    <row r="47" spans="4:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D47" s="55"/>
       <c r="E47" s="56"/>
       <c r="F47" s="57"/>
@@ -4527,7 +4528,7 @@
       <c r="X47" s="42"/>
       <c r="Y47" s="25"/>
     </row>
-    <row r="48" spans="4:25">
+    <row r="48" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D48" s="55"/>
       <c r="E48" s="58"/>
       <c r="F48" s="57"/>
@@ -4547,7 +4548,7 @@
       <c r="X48" s="42"/>
       <c r="Y48" s="25"/>
     </row>
-    <row r="49" spans="4:25">
+    <row r="49" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D49" s="55"/>
       <c r="E49" s="56"/>
       <c r="F49" s="57"/>
@@ -4567,7 +4568,7 @@
       <c r="X49" s="42"/>
       <c r="Y49" s="25"/>
     </row>
-    <row r="50" spans="4:25">
+    <row r="50" spans="4:25" x14ac:dyDescent="0.2">
       <c r="O50" s="41" t="s">
         <v>285</v>
       </c>
@@ -4584,7 +4585,7 @@
       <c r="X50" s="42"/>
       <c r="Y50" s="25"/>
     </row>
-    <row r="51" spans="4:25">
+    <row r="51" spans="4:25" x14ac:dyDescent="0.2">
       <c r="Q51" s="25"/>
       <c r="R51" s="25"/>
       <c r="T51" s="25"/>
@@ -4594,7 +4595,7 @@
       <c r="X51" s="25"/>
       <c r="Y51" s="25"/>
     </row>
-    <row r="52" spans="4:25">
+    <row r="52" spans="4:25" x14ac:dyDescent="0.2">
       <c r="Q52" s="25"/>
       <c r="R52" s="25"/>
       <c r="T52" s="25"/>
@@ -4604,7 +4605,7 @@
       <c r="X52" s="25"/>
       <c r="Y52" s="25"/>
     </row>
-    <row r="53" spans="4:25">
+    <row r="53" spans="4:25" x14ac:dyDescent="0.2">
       <c r="Q53" s="25"/>
       <c r="R53" s="25"/>
       <c r="T53" s="25"/>
@@ -4614,7 +4615,7 @@
       <c r="X53" s="25"/>
       <c r="Y53" s="25"/>
     </row>
-    <row r="54" spans="4:25">
+    <row r="54" spans="4:25" x14ac:dyDescent="0.2">
       <c r="P54" s="25"/>
       <c r="Q54" s="25"/>
       <c r="R54" s="25"/>
@@ -4625,7 +4626,7 @@
       <c r="X54" s="25"/>
       <c r="Y54" s="25"/>
     </row>
-    <row r="55" spans="4:25">
+    <row r="55" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D55" s="59"/>
       <c r="P55" s="25"/>
       <c r="Q55" s="25"/>
@@ -4637,7 +4638,7 @@
       <c r="X55" s="25"/>
       <c r="Y55" s="25"/>
     </row>
-    <row r="56" spans="4:25">
+    <row r="56" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D56" s="59"/>
       <c r="H56" s="53"/>
       <c r="P56" s="25"/>
@@ -4650,7 +4651,7 @@
       <c r="X56" s="25"/>
       <c r="Y56" s="25"/>
     </row>
-    <row r="57" spans="4:25">
+    <row r="57" spans="4:25" x14ac:dyDescent="0.2">
       <c r="H57" s="53"/>
       <c r="P57" s="25"/>
       <c r="Q57" s="25"/>
@@ -4662,7 +4663,7 @@
       <c r="X57" s="25"/>
       <c r="Y57" s="25"/>
     </row>
-    <row r="58" spans="4:25">
+    <row r="58" spans="4:25" x14ac:dyDescent="0.2">
       <c r="P58" s="25"/>
       <c r="Q58" s="25"/>
       <c r="R58" s="25"/>
@@ -4673,7 +4674,7 @@
       <c r="X58" s="25"/>
       <c r="Y58" s="25"/>
     </row>
-    <row r="59" spans="4:25">
+    <row r="59" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D59" s="59"/>
       <c r="P59" s="25"/>
       <c r="Q59" s="25"/>
@@ -4685,7 +4686,7 @@
       <c r="X59" s="25"/>
       <c r="Y59" s="25"/>
     </row>
-    <row r="60" spans="4:25">
+    <row r="60" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D60" s="59"/>
       <c r="P60" s="25"/>
       <c r="Q60" s="25"/>
@@ -4697,7 +4698,7 @@
       <c r="X60" s="25"/>
       <c r="Y60" s="25"/>
     </row>
-    <row r="61" spans="4:25">
+    <row r="61" spans="4:25" x14ac:dyDescent="0.2">
       <c r="D61" s="59"/>
       <c r="P61" s="25"/>
       <c r="Q61" s="25"/>
@@ -4709,7 +4710,7 @@
       <c r="X61" s="25"/>
       <c r="Y61" s="25"/>
     </row>
-    <row r="62" spans="4:25">
+    <row r="62" spans="4:25" x14ac:dyDescent="0.2">
       <c r="P62" s="25"/>
       <c r="Q62" s="25"/>
       <c r="R62" s="25"/>
@@ -4720,7 +4721,7 @@
       <c r="X62" s="25"/>
       <c r="Y62" s="25"/>
     </row>
-    <row r="63" spans="4:25">
+    <row r="63" spans="4:25" x14ac:dyDescent="0.2">
       <c r="P63" s="25"/>
       <c r="Q63" s="25"/>
       <c r="R63" s="25"/>
@@ -4731,7 +4732,7 @@
       <c r="X63" s="25"/>
       <c r="Y63" s="25"/>
     </row>
-    <row r="64" spans="4:25">
+    <row r="64" spans="4:25" x14ac:dyDescent="0.2">
       <c r="P64" s="25"/>
       <c r="Q64" s="25"/>
       <c r="R64" s="25"/>
@@ -4742,7 +4743,7 @@
       <c r="X64" s="25"/>
       <c r="Y64" s="25"/>
     </row>
-    <row r="65" spans="4:23">
+    <row r="65" spans="4:23" x14ac:dyDescent="0.2">
       <c r="P65" s="25"/>
       <c r="Q65" s="25"/>
       <c r="R65" s="25"/>
@@ -4751,70 +4752,65 @@
       <c r="V65" s="25"/>
       <c r="W65" s="25"/>
     </row>
-    <row r="66" spans="4:23">
+    <row r="66" spans="4:23" x14ac:dyDescent="0.2">
       <c r="Q66" s="25"/>
       <c r="V66" s="25"/>
       <c r="W66" s="25"/>
     </row>
-    <row r="67" spans="4:23">
+    <row r="67" spans="4:23" x14ac:dyDescent="0.2">
       <c r="Q67" s="25"/>
       <c r="V67" s="25"/>
       <c r="W67" s="25"/>
     </row>
-    <row r="72" spans="4:23">
+    <row r="72" spans="4:23" x14ac:dyDescent="0.2">
       <c r="D72" s="60"/>
       <c r="E72" s="60"/>
       <c r="F72" s="60"/>
     </row>
-    <row r="73" spans="4:23">
+    <row r="73" spans="4:23" x14ac:dyDescent="0.2">
       <c r="D73" s="61"/>
       <c r="E73" s="62"/>
       <c r="F73" s="63"/>
     </row>
-    <row r="74" spans="4:23">
+    <row r="74" spans="4:23" x14ac:dyDescent="0.2">
       <c r="D74" s="61"/>
       <c r="E74" s="62"/>
       <c r="F74" s="63"/>
     </row>
-    <row r="75" spans="4:23">
+    <row r="75" spans="4:23" x14ac:dyDescent="0.2">
       <c r="D75" s="61"/>
       <c r="E75" s="62"/>
       <c r="F75" s="63"/>
     </row>
-    <row r="76" spans="4:23">
+    <row r="76" spans="4:23" x14ac:dyDescent="0.2">
       <c r="D76" s="61"/>
       <c r="E76" s="62"/>
       <c r="F76" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="O4:Y4"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H12:H15"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="H27:H31"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="O4:Y4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H4:M4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4826,7 +4822,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
@@ -4834,7 +4830,7 @@
     <col min="4" max="4" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>170</v>
       </c>
@@ -4848,7 +4844,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="65" customFormat="1">
+    <row r="2" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="75">
         <v>42223</v>
       </c>
@@ -4860,7 +4856,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="65" customFormat="1">
+    <row r="3" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="75"/>
       <c r="B3" s="107"/>
       <c r="C3" s="107"/>
@@ -4868,13 +4864,13 @@
         <v>377</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="65" customFormat="1">
+    <row r="4" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="108"/>
       <c r="B4" s="109"/>
       <c r="C4" s="109"/>
       <c r="D4" s="109"/>
     </row>
-    <row r="5" spans="1:4" s="65" customFormat="1">
+    <row r="5" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="75">
         <v>42179</v>
       </c>
@@ -4886,7 +4882,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="65" customFormat="1">
+    <row r="6" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="75"/>
       <c r="B6" s="107"/>
       <c r="C6" s="107"/>
@@ -4894,7 +4890,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="65" customFormat="1">
+    <row r="7" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="75"/>
       <c r="B7" s="107"/>
       <c r="C7" s="107"/>
@@ -4902,7 +4898,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="65" customFormat="1">
+    <row r="8" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="75"/>
       <c r="B8" s="107"/>
       <c r="C8" s="107"/>
@@ -4910,7 +4906,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="65" customFormat="1">
+    <row r="9" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="107"/>
       <c r="C9" s="107"/>
@@ -4918,7 +4914,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="65" customFormat="1">
+    <row r="10" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="75"/>
       <c r="B10" s="107"/>
       <c r="C10" s="107"/>
@@ -4926,7 +4922,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="65" customFormat="1">
+    <row r="11" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="75"/>
       <c r="B11" s="107"/>
       <c r="C11" s="107"/>
@@ -4934,7 +4930,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="65" customFormat="1">
+    <row r="12" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="75"/>
       <c r="B12" s="107"/>
       <c r="C12" s="107"/>
@@ -4942,7 +4938,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="65" customFormat="1">
+    <row r="13" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="75"/>
       <c r="B13" s="107"/>
       <c r="C13" s="107"/>
@@ -4950,7 +4946,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="65" customFormat="1">
+    <row r="14" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="75"/>
       <c r="B14" s="107"/>
       <c r="C14" s="107"/>
@@ -4958,7 +4954,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="65" customFormat="1">
+    <row r="15" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="75"/>
       <c r="B15" s="107"/>
       <c r="C15" s="107"/>
@@ -4966,13 +4962,13 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="65" customFormat="1">
+    <row r="16" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" s="74" customFormat="1">
+    <row r="17" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="75">
         <v>42165</v>
       </c>
@@ -4986,91 +4982,91 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="74" customFormat="1">
+    <row r="18" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" s="78" customFormat="1">
+    <row r="19" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" s="74" customFormat="1">
+    <row r="20" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" s="74" customFormat="1">
+    <row r="21" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" s="74" customFormat="1">
+    <row r="22" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" s="74" customFormat="1">
+    <row r="23" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" s="74" customFormat="1">
+    <row r="24" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" s="74" customFormat="1">
+    <row r="25" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" s="74" customFormat="1">
+    <row r="26" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" s="74" customFormat="1">
+    <row r="27" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" s="78" customFormat="1">
+    <row r="28" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" s="76" customFormat="1">
+    <row r="29" spans="1:4" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" s="78" customFormat="1">
+    <row r="30" spans="1:4" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" s="74" customFormat="1">
+    <row r="31" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" s="65" customFormat="1">
+    <row r="32" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -5080,11 +5076,6 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5096,707 +5087,707 @@
       <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="105.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="101" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="102" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="103" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="103" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="93" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="93" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="93" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="103" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="103" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="103" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="93" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="93" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="93" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="103" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="103" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="103" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="93" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="93" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="93" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="103" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="103" t="s">
         <v>340</v>
       </c>
@@ -5805,11 +5796,6 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5819,14 +5805,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>209</v>
       </c>
@@ -5837,7 +5823,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -5848,7 +5834,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -5859,7 +5845,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -5870,7 +5856,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -5881,7 +5867,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="65" customFormat="1">
+    <row r="6" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="65" t="s">
         <v>231</v>
       </c>
@@ -5892,7 +5878,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>215</v>
       </c>
@@ -5903,7 +5889,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -5914,7 +5900,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -5925,7 +5911,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>216</v>
       </c>
@@ -5936,7 +5922,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>217</v>
       </c>
@@ -5947,7 +5933,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="65" t="s">
         <v>229</v>
       </c>
@@ -5960,10 +5946,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>